<commit_message>
architecture + tableau en cours
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicopatsch/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theoc\Desktop\p4 OCR\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAECDB4-2AAF-41CB-AF7E-B4CCA154AC19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="620" windowWidth="27860" windowHeight="17380" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
   <si>
     <t>Catégorie</t>
   </si>
@@ -51,13 +52,145 @@
   </si>
   <si>
     <t>(SEO ou accessiblité ?)</t>
+  </si>
+  <si>
+    <t>SEO</t>
+  </si>
+  <si>
+    <t>lang="Default"</t>
+  </si>
+  <si>
+    <t>Le site est en français, il faut le mettre en fr</t>
+  </si>
+  <si>
+    <t>w3c</t>
+  </si>
+  <si>
+    <t>Le titre sert a se repérer pour savoir sur quelle page on est</t>
+  </si>
+  <si>
+    <t>opquast</t>
+  </si>
+  <si>
+    <t>Accessibilité</t>
+  </si>
+  <si>
+    <t>non voyant</t>
+  </si>
+  <si>
+    <t>Utiliser des moyens permettant aux non voyants d'aller sur le site</t>
+  </si>
+  <si>
+    <t>utiliser des alt pour les images</t>
+  </si>
+  <si>
+    <t>Amérliorer le visuel</t>
+  </si>
+  <si>
+    <t>Couleurs / tailles images  etc..</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>OCR</t>
+  </si>
+  <si>
+    <t>Balise canonique</t>
+  </si>
+  <si>
+    <t>permet un meilleur référencement</t>
+  </si>
+  <si>
+    <t>Allègement image</t>
+  </si>
+  <si>
+    <t>rapidité du site via des images compressées</t>
+  </si>
+  <si>
+    <t>Minification JS / CSS</t>
+  </si>
+  <si>
+    <t>Permet un allègement du poids de ces fichiers</t>
+  </si>
+  <si>
+    <t>Structuration du code HTML</t>
+  </si>
+  <si>
+    <t>Permet un référencement naturel</t>
+  </si>
+  <si>
+    <t>Responsive</t>
+  </si>
+  <si>
+    <t>Le site est très peu responsive</t>
+  </si>
+  <si>
+    <t>Permettre un accès sur tablette et mobile plus simplifié</t>
+  </si>
+  <si>
+    <t>Meta</t>
+  </si>
+  <si>
+    <t>Balises meta mal utilisées</t>
+  </si>
+  <si>
+    <t>Référencement naturel</t>
+  </si>
+  <si>
+    <t>sitemap et robot.txt</t>
+  </si>
+  <si>
+    <t>pas de fichier</t>
+  </si>
+  <si>
+    <t>permet un lecture plus rapide par le bot google</t>
+  </si>
+  <si>
+    <t>Utiliser son code pour référencer naturellement (que des divs ici)</t>
+  </si>
+  <si>
+    <t>title + ordre balise (h1,h2 etc)</t>
+  </si>
+  <si>
+    <t>pas de balise label html2</t>
+  </si>
+  <si>
+    <t>erreur</t>
+  </si>
+  <si>
+    <t>html2 &gt; contact.html</t>
+  </si>
+  <si>
+    <t>renomage de fichier / titre</t>
+  </si>
+  <si>
+    <t>permet une meilleure lisibilité</t>
+  </si>
+  <si>
+    <t>utiliser du texte pas d'image</t>
+  </si>
+  <si>
+    <t>la quote devrait être utilisée en texte.</t>
+  </si>
+  <si>
+    <t>rapidité</t>
+  </si>
+  <si>
+    <t>balise meta description vide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">première chose qu'on voit sur le site vide </t>
+  </si>
+  <si>
+    <t>meilleur lisibilité</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -86,6 +219,17 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -122,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -130,6 +274,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -139,6 +285,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -341,22 +490,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
-    <col min="7" max="26" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="3" max="4" width="51.109375" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" customWidth="1"/>
+    <col min="7" max="26" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -396,68 +547,265 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
       <c r="E3" s="4"/>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
       <c r="E4" s="4"/>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E5" s="4"/>
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E6" s="4"/>
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E7" s="4"/>
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E8" s="4"/>
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E9" s="4"/>
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E10" s="4"/>
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E11" s="4"/>
+    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E12" s="4"/>
+    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E15" s="4"/>
+    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1428,6 +1776,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>